<commit_message>
modifications to the spreadsheet
</commit_message>
<xml_diff>
--- a/STARCRAFT STATS 4.1.xlsx
+++ b/STARCRAFT STATS 4.1.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23416"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UW\Projects\StarcraftStats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16425"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Overall Stats" sheetId="14" r:id="rId2"/>
     <sheet name="Match Up Stats" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -491,16 +496,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,18 +524,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,16 +538,554 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+  <dxfs count="118">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -558,6 +1101,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -573,6 +1126,586 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -629,7 +1762,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -683,13 +1815,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -742,13 +1874,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -793,13 +1925,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -852,13 +1984,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -908,13 +2040,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -967,13 +2099,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,11 +2120,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2076873976"/>
-        <c:axId val="2076877000"/>
+        <c:axId val="123972096"/>
+        <c:axId val="123972656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076873976"/>
+        <c:axId val="123972096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +2134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076877000"/>
+        <c:crossAx val="123972656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +2142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076877000"/>
+        <c:axId val="123972656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,15 +2153,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076873976"/>
+        <c:crossAx val="123972096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1069,7 +2200,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1141,31 +2271,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1236,31 +2366,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1323,31 +2453,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,31 +2548,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,31 +2640,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1605,31 +2735,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1644,11 +2774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2076946648"/>
-        <c:axId val="2076949672"/>
+        <c:axId val="125364512"/>
+        <c:axId val="125365072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076946648"/>
+        <c:axId val="125364512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +2788,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076949672"/>
+        <c:crossAx val="125365072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1666,7 +2796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076949672"/>
+        <c:axId val="125365072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,15 +2807,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076946648"/>
+        <c:crossAx val="125364512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2060,67 +3189,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.42578125" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.5" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.42578125" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.1640625" customWidth="1"/>
-    <col min="41" max="41" width="9.1640625" customWidth="1"/>
-    <col min="42" max="43" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" customWidth="1"/>
+    <col min="42" max="43" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="14" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="21" thickBot="1">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:57" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
     </row>
-    <row r="2" spans="1:57">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
@@ -2157,24 +3286,24 @@
       <c r="L2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="X2" s="41" t="s">
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="X2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
     </row>
-    <row r="3" spans="1:57">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2214,28 +3343,28 @@
         <f>SUM(J3:K3)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="41" t="s">
+      <c r="O3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41" t="s">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="X3" s="41" t="s">
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="X3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41" t="s">
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
     </row>
-    <row r="4" spans="1:57" ht="15" thickBot="1">
+    <row r="4" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
@@ -2314,9 +3443,9 @@
       <c r="AP4" s="16"/>
       <c r="AQ4" s="16"/>
       <c r="AR4" s="16"/>
-      <c r="AS4" s="41"/>
-      <c r="AT4" s="41"/>
-      <c r="AU4" s="41"/>
+      <c r="AS4" s="38"/>
+      <c r="AT4" s="38"/>
+      <c r="AU4" s="38"/>
       <c r="AW4" s="16"/>
       <c r="AX4" s="16"/>
       <c r="AY4" s="16"/>
@@ -2327,7 +3456,7 @@
       <c r="BD4" s="16"/>
       <c r="BE4" s="16"/>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>16</v>
       </c>
@@ -2367,10 +3496,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="39" t="s">
         <v>1</v>
       </c>
       <c r="O5" s="6">
@@ -2397,13 +3526,13 @@
         <f>K8</f>
         <v>0</v>
       </c>
-      <c r="U5" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="V5" s="35" t="s">
+      <c r="U5" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="V5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="W5" s="36" t="s">
+      <c r="W5" s="39" t="s">
         <v>1</v>
       </c>
       <c r="X5" s="11">
@@ -2430,10 +3559,10 @@
         <f>IF(SUM(J8:K8)=0,0,K8/SUM(J8:K8))</f>
         <v>0</v>
       </c>
-      <c r="AD5" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="35" t="s">
+      <c r="AD5" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="AS5" t="s">
@@ -2473,7 +3602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="15" thickBot="1">
+    <row r="6" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
@@ -2513,8 +3642,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="36"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="39"/>
       <c r="O6" s="8">
         <f>B13</f>
         <v>0</v>
@@ -2539,9 +3668,9 @@
         <f>J8</f>
         <v>0</v>
       </c>
-      <c r="U6" s="38"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="36"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="39"/>
       <c r="X6" s="13">
         <f>IF(SUM(B13:C13)=0,0,B13/SUM(B13:C13))</f>
         <v>0</v>
@@ -2566,8 +3695,8 @@
         <f>IF(SUM(J8:K8)=0,0,J8/SUM(J8:K8))</f>
         <v>0</v>
       </c>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="35"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="43"/>
       <c r="AR6" t="s">
         <v>41</v>
       </c>
@@ -2623,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>18</v>
       </c>
@@ -2663,8 +3792,8 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="M7" s="35"/>
-      <c r="N7" s="36" t="s">
+      <c r="M7" s="43"/>
+      <c r="N7" s="39" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="6">
@@ -2691,11 +3820,11 @@
         <f>K3</f>
         <v>0</v>
       </c>
-      <c r="U7" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="V7" s="35"/>
-      <c r="W7" s="36" t="s">
+      <c r="U7" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="43"/>
+      <c r="W7" s="39" t="s">
         <v>0</v>
       </c>
       <c r="X7" s="11">
@@ -2722,10 +3851,10 @@
         <f>IF(SUM(J3:K3)=0,0,K3/SUM(J3:K3))</f>
         <v>0</v>
       </c>
-      <c r="AD7" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="35"/>
+      <c r="AD7" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="43"/>
       <c r="AR7" t="s">
         <v>38</v>
       </c>
@@ -2781,7 +3910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="15" thickBot="1">
+    <row r="8" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>19</v>
       </c>
@@ -2821,8 +3950,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="35"/>
-      <c r="N8" s="36"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="39"/>
       <c r="O8" s="8">
         <f>B4</f>
         <v>0</v>
@@ -2847,9 +3976,9 @@
         <f>K4</f>
         <v>1</v>
       </c>
-      <c r="U8" s="38"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="36"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="39"/>
       <c r="X8" s="13">
         <f>IF(SUM(B4:C4)=0,0,B4/SUM(B4:C4))</f>
         <v>0</v>
@@ -2874,8 +4003,8 @@
         <f>IF(SUM(J3:K3)=0,0,J3/SUM(J3:K3))</f>
         <v>0</v>
       </c>
-      <c r="AD8" s="37"/>
-      <c r="AE8" s="35"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="43"/>
       <c r="AR8" t="s">
         <v>42</v>
       </c>
@@ -2931,7 +4060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:57">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -2944,8 +4073,8 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="36" t="s">
+      <c r="M9" s="43"/>
+      <c r="N9" s="39" t="s">
         <v>2</v>
       </c>
       <c r="O9" s="6">
@@ -2972,11 +4101,11 @@
         <f>K12</f>
         <v>0</v>
       </c>
-      <c r="U9" s="38" t="s">
+      <c r="U9" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="V9" s="35"/>
-      <c r="W9" s="36" t="s">
+      <c r="V9" s="43"/>
+      <c r="W9" s="39" t="s">
         <v>2</v>
       </c>
       <c r="X9" s="11">
@@ -3003,10 +4132,10 @@
         <f>IF(SUM(J12:K12)=0,0,K12/SUM(J12:K12))</f>
         <v>0</v>
       </c>
-      <c r="AD9" s="38" t="s">
+      <c r="AD9" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="AE9" s="35"/>
+      <c r="AE9" s="43"/>
       <c r="AR9" t="s">
         <v>39</v>
       </c>
@@ -3062,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:57" ht="15" thickBot="1">
+    <row r="10" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
@@ -3081,8 +4210,8 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="36"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="39"/>
       <c r="O10" s="8">
         <f>B6</f>
         <v>0</v>
@@ -3107,9 +4236,9 @@
         <f>J12</f>
         <v>0</v>
       </c>
-      <c r="U10" s="38"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="36"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="39"/>
       <c r="X10" s="13">
         <f>IF(SUM(B6:C6)=0,0,B6/SUM(B6:C6))</f>
         <v>0</v>
@@ -3134,8 +4263,8 @@
         <f>IF(SUM(J12:K12)=0,0,J12/SUM(J12:K12))</f>
         <v>0</v>
       </c>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="35"/>
+      <c r="AD10" s="40"/>
+      <c r="AE10" s="43"/>
       <c r="AR10" t="s">
         <v>43</v>
       </c>
@@ -3191,7 +4320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:57">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>20</v>
       </c>
@@ -3231,10 +4360,10 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P11" s="39" t="s">
+      <c r="P11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="Q11" s="40" t="s">
+      <c r="Q11" s="42" t="s">
         <v>1</v>
       </c>
       <c r="R11" s="6">
@@ -3249,16 +4378,16 @@
         <f>G8</f>
         <v>0</v>
       </c>
-      <c r="U11" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="V11" s="35" t="s">
+      <c r="U11" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="Y11" s="39" t="s">
+      <c r="Y11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="Z11" s="40" t="s">
+      <c r="Z11" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AA11" s="11">
@@ -3273,10 +4402,10 @@
         <f>IF(SUM(F8:G8)=0,0,G8/SUM(F8:G8))</f>
         <v>0</v>
       </c>
-      <c r="AD11" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="35" t="s">
+      <c r="AD11" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="43" t="s">
         <v>5</v>
       </c>
       <c r="AR11" t="s">
@@ -3334,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="15" thickBot="1">
+    <row r="12" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>21</v>
       </c>
@@ -3374,8 +4503,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="36"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="39"/>
       <c r="R12" s="8">
         <f>F13</f>
         <v>1</v>
@@ -3388,10 +4517,10 @@
         <f>F8</f>
         <v>0</v>
       </c>
-      <c r="U12" s="38"/>
-      <c r="V12" s="35"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="36"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="39"/>
       <c r="AA12" s="13">
         <f>IF(SUM(F13:G13)=0,0,F13/SUM(F13:G13))</f>
         <v>1</v>
@@ -3404,10 +4533,10 @@
         <f>IF(SUM(F8:G8)=0,0,F8/SUM(F8:G8))</f>
         <v>0</v>
       </c>
-      <c r="AD12" s="38"/>
-      <c r="AE12" s="35"/>
+      <c r="AD12" s="40"/>
+      <c r="AE12" s="43"/>
     </row>
-    <row r="13" spans="1:57">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>22</v>
       </c>
@@ -3447,8 +4576,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="36" t="s">
+      <c r="P13" s="40"/>
+      <c r="Q13" s="39" t="s">
         <v>0</v>
       </c>
       <c r="R13" s="6">
@@ -3463,12 +4592,12 @@
         <f>G3</f>
         <v>0</v>
       </c>
-      <c r="U13" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="V13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="36" t="s">
+      <c r="U13" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="V13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="39" t="s">
         <v>0</v>
       </c>
       <c r="AA13" s="11">
@@ -3483,12 +4612,12 @@
         <f>IF(SUM(F3:G3)=0,0,G3/SUM(F3:G3))</f>
         <v>0</v>
       </c>
-      <c r="AD13" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="35"/>
+      <c r="AD13" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="43"/>
     </row>
-    <row r="14" spans="1:57" ht="15" thickBot="1">
+    <row r="14" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -3501,8 +4630,8 @@
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="3"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="36"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="39"/>
       <c r="R14" s="8">
         <f>F4</f>
         <v>0</v>
@@ -3515,10 +4644,10 @@
         <f>F3</f>
         <v>0</v>
       </c>
-      <c r="U14" s="38"/>
-      <c r="V14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="36"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="39"/>
       <c r="AA14" s="13">
         <f>IF(SUM(F4:G4)=0,0,F4/SUM(F4:G4))</f>
         <v>0</v>
@@ -3531,10 +4660,10 @@
         <f>IF(SUM(F3:G3)=0,0,F3/SUM(F3:G3))</f>
         <v>0</v>
       </c>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="35"/>
+      <c r="AD14" s="40"/>
+      <c r="AE14" s="43"/>
     </row>
-    <row r="15" spans="1:57" ht="15" thickBot="1">
+    <row r="15" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>24</v>
       </c>
@@ -3580,8 +4709,8 @@
         <f>SUM(L3:L13)</f>
         <v>11</v>
       </c>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="36" t="s">
+      <c r="P15" s="40"/>
+      <c r="Q15" s="39" t="s">
         <v>2</v>
       </c>
       <c r="R15" s="6">
@@ -3596,12 +4725,12 @@
         <f>G12</f>
         <v>0</v>
       </c>
-      <c r="U15" s="37" t="s">
+      <c r="U15" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="V15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="36" t="s">
+      <c r="V15" s="43"/>
+      <c r="Y15" s="43"/>
+      <c r="Z15" s="39" t="s">
         <v>2</v>
       </c>
       <c r="AA15" s="11">
@@ -3616,14 +4745,14 @@
         <f>IF(SUM(F12:G12)=0,0,G12/SUM(F12:G12))</f>
         <v>0</v>
       </c>
-      <c r="AD15" s="38" t="s">
+      <c r="AD15" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="AE15" s="35"/>
+      <c r="AE15" s="43"/>
     </row>
-    <row r="16" spans="1:57" ht="15" thickBot="1">
-      <c r="P16" s="38"/>
-      <c r="Q16" s="36"/>
+    <row r="16" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P16" s="40"/>
+      <c r="Q16" s="39"/>
       <c r="R16" s="5">
         <f>F6</f>
         <v>0</v>
@@ -3636,10 +4765,10 @@
         <f>F12</f>
         <v>0</v>
       </c>
-      <c r="U16" s="37"/>
-      <c r="V16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="36"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="43"/>
+      <c r="Y16" s="43"/>
+      <c r="Z16" s="39"/>
       <c r="AA16" s="15">
         <f>IF(SUM(F6:G6)=0,0,F6/SUM(F6:G6))</f>
         <v>0</v>
@@ -3652,27 +4781,27 @@
         <f>IF(SUM(F12:G12)=0,0,F12/SUM(F12:G12))</f>
         <v>0</v>
       </c>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="35"/>
+      <c r="AD16" s="40"/>
+      <c r="AE16" s="43"/>
     </row>
-    <row r="19" spans="14:25" ht="15" thickBot="1"/>
-    <row r="20" spans="14:25">
-      <c r="N20" s="43" t="s">
+    <row r="19" spans="14:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="14:25" x14ac:dyDescent="0.25">
+      <c r="N20" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
-      <c r="Q20" s="44"/>
-      <c r="R20" s="44"/>
-      <c r="S20" s="44"/>
-      <c r="T20" s="44"/>
-      <c r="U20" s="44"/>
-      <c r="V20" s="44"/>
-      <c r="W20" s="44"/>
-      <c r="X20" s="44"/>
-      <c r="Y20" s="45"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="37"/>
     </row>
-    <row r="21" spans="14:25">
+    <row r="21" spans="14:25" x14ac:dyDescent="0.25">
       <c r="N21" s="18" t="s">
         <v>24</v>
       </c>
@@ -3683,21 +4812,21 @@
       <c r="P21" s="17"/>
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
-      <c r="S21" s="42" t="s">
+      <c r="S21" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="42" t="s">
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="W21" s="42"/>
-      <c r="X21" s="42"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
       <c r="Y21" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="14:25">
+    <row r="22" spans="14:25" x14ac:dyDescent="0.25">
       <c r="N22" s="18"/>
       <c r="O22" s="17" t="s">
         <v>26</v>
@@ -3731,7 +4860,7 @@
       </c>
       <c r="Y22" s="32"/>
     </row>
-    <row r="23" spans="14:25">
+    <row r="23" spans="14:25" x14ac:dyDescent="0.25">
       <c r="N23" s="18" t="s">
         <v>5</v>
       </c>
@@ -3780,7 +4909,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="24" spans="14:25">
+    <row r="24" spans="14:25" x14ac:dyDescent="0.25">
       <c r="N24" s="18" t="s">
         <v>6</v>
       </c>
@@ -3829,7 +4958,7 @@
         <v>P</v>
       </c>
     </row>
-    <row r="25" spans="14:25" ht="15" thickBot="1">
+    <row r="25" spans="14:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N25" s="19" t="s">
         <v>7</v>
       </c>
@@ -3880,6 +5009,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="AE5:AE10"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="M5:M10"/>
+    <mergeCell ref="X2:AC2"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="V11:V16"/>
+    <mergeCell ref="V5:V10"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AC3"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
     <mergeCell ref="S21:U21"/>
     <mergeCell ref="V21:X21"/>
     <mergeCell ref="N20:Y20"/>
@@ -3891,63 +5046,292 @@
     <mergeCell ref="U9:U10"/>
     <mergeCell ref="P11:P16"/>
     <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
     <mergeCell ref="Y11:Y16"/>
     <mergeCell ref="Z11:Z12"/>
     <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="V11:V16"/>
-    <mergeCell ref="V5:V10"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="W5:W6"/>
     <mergeCell ref="AE11:AE16"/>
-    <mergeCell ref="Z13:Z14"/>
     <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="AE5:AE10"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="M5:M10"/>
   </mergeCells>
-  <conditionalFormatting sqref="X5:AC10">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="X5:AC10 AA11:AC16">
+    <cfRule type="cellIs" dxfId="114" priority="57" operator="equal">
       <formula>0.5</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA11:AC16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="56" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X5:AC10 Y11:AC16">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X5:AC16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="X5">
+    <cfRule type="expression" dxfId="112" priority="55">
+      <formula>AND($X$5&lt;0.5,SUM($X$5:$X$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X6">
+    <cfRule type="expression" dxfId="111" priority="53">
+      <formula>AND($X$6&lt;0.5,SUM($X$5:$X$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X7">
+    <cfRule type="expression" dxfId="110" priority="52">
+      <formula>AND($X$7&lt;0.5,SUM($X$7:$X$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X8">
+    <cfRule type="expression" dxfId="109" priority="51">
+      <formula>AND($X$8&lt;0.5,SUM($X$7:$X$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X9">
+    <cfRule type="expression" dxfId="108" priority="50">
+      <formula>AND($X$9&lt;0.5,SUM($X$9:$X$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X10">
+    <cfRule type="expression" dxfId="107" priority="49">
+      <formula>AND($X$10&lt;0.5,SUM($X$9:$X$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y5">
+    <cfRule type="expression" dxfId="106" priority="48">
+      <formula>AND($Y$5&lt;0.5,SUM($Y$5:$Y$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y6">
+    <cfRule type="expression" dxfId="105" priority="47">
+      <formula>AND($Y$6&lt;0.5,SUM($Y$5:$Y$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y7">
+    <cfRule type="expression" dxfId="104" priority="46">
+      <formula>AND($Y$7&lt;0.5,SUM($Y$7:$Y$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y8">
+    <cfRule type="expression" dxfId="103" priority="45">
+      <formula>AND($Y$8&lt;0.5,SUM($Y$7:$Y$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y9">
+    <cfRule type="expression" dxfId="102" priority="44">
+      <formula>AND($Y$9&lt;0.5,SUM($Y$9:$Y$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y10">
+    <cfRule type="expression" dxfId="101" priority="43">
+      <formula>AND($Y$10&lt;0.5,SUM($Y$9:$Y$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z5">
+    <cfRule type="expression" dxfId="100" priority="42">
+      <formula>AND($Z$5&lt;0.5,SUM($Z$5:$Z$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z6">
+    <cfRule type="expression" dxfId="99" priority="41">
+      <formula>AND($Z$6&lt;0.5,SUM($Z$5:$Z$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z7">
+    <cfRule type="expression" dxfId="98" priority="40">
+      <formula>AND($Z$7&lt;0.5,SUM($Z$7:$Z$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z8">
+    <cfRule type="expression" dxfId="97" priority="39">
+      <formula>AND($Z$8&lt;0.5,SUM($Z$7:$Z$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z9">
+    <cfRule type="expression" dxfId="96" priority="38">
+      <formula>AND($Z$9&lt;0.5,SUM($Z$9:$Z$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z10">
+    <cfRule type="expression" dxfId="95" priority="37">
+      <formula>AND($Z$10&lt;0.5,SUM($Z$9:$Z$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA5">
+    <cfRule type="expression" dxfId="94" priority="36">
+      <formula>AND($AA$5&lt;0.5,SUM($AA$5:$AA$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA6">
+    <cfRule type="expression" dxfId="93" priority="35">
+      <formula>AND($AA$6&lt;0.5,SUM($AA$5:$AA$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA7">
+    <cfRule type="expression" dxfId="92" priority="34">
+      <formula>AND($AA$7&lt;0.5,SUM($AA$7:$AA$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA8">
+    <cfRule type="expression" dxfId="91" priority="33">
+      <formula>AND($AA$8&lt;0.5,SUM($AA$7:$AA$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA9">
+    <cfRule type="expression" dxfId="90" priority="32">
+      <formula>AND($AA$9&lt;0.5,SUM($AA$9:$AA$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA10">
+    <cfRule type="expression" dxfId="59" priority="31">
+      <formula>AND($AA$10&lt;0.5,SUM($AA$9:$AA$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA11">
+    <cfRule type="expression" dxfId="89" priority="30">
+      <formula>AND($AA$11&lt;0.5,SUM($AA$11:$AA$12)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA12">
+    <cfRule type="expression" dxfId="88" priority="29">
+      <formula>AND($AA$12&lt;0.5,SUM($AA$11:$AA$12)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA13">
+    <cfRule type="expression" dxfId="87" priority="28">
+      <formula>AND($AA$13&lt;0.5,SUM($AA$13:$AA$14)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA14">
+    <cfRule type="expression" dxfId="86" priority="27">
+      <formula>AND($AA$14&lt;0.5,SUM($AA$13:$AA$14)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA15">
+    <cfRule type="expression" dxfId="85" priority="26">
+      <formula>AND($AA$15&lt;0.5,SUM($AA$15:$AA$16)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA16">
+    <cfRule type="expression" dxfId="84" priority="25">
+      <formula>AND($AA$16&lt;0.5,SUM($AA$15:$AA$16)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB5">
+    <cfRule type="expression" dxfId="83" priority="24">
+      <formula>AND($AB$5&lt;0.5,SUM($AB$5:$AB$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB6">
+    <cfRule type="expression" dxfId="82" priority="23">
+      <formula>AND($AB$6&lt;0.5,SUM($AB$5:$AB$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB7">
+    <cfRule type="expression" dxfId="81" priority="22">
+      <formula>AND($AB$7&lt;0.5,SUM($AB$7:$AB$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB8">
+    <cfRule type="expression" dxfId="80" priority="21">
+      <formula>AND($AB$8&lt;0.5,SUM($AB$7:$AB$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB9">
+    <cfRule type="expression" dxfId="79" priority="20">
+      <formula>AND($AB$9&lt;0.5,SUM($AB$9:$AB$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB10">
+    <cfRule type="expression" dxfId="78" priority="19">
+      <formula>AND($AB$10&lt;0.5,SUM($AB$9:$AB$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB11">
+    <cfRule type="expression" dxfId="77" priority="18">
+      <formula>AND($AB$11&lt;0.5,SUM($AB$11:$AB$12)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB12">
+    <cfRule type="expression" dxfId="76" priority="17">
+      <formula>AND($AB$12&lt;0.5,SUM($AB$11:$AB$12)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB13">
+    <cfRule type="expression" dxfId="75" priority="16">
+      <formula>AND($AB$13&lt;0.5,SUM($AB$13:$AB$14)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB14">
+    <cfRule type="expression" dxfId="74" priority="15">
+      <formula>AND($AB$14&lt;0.5,SUM($AB$13:$AB$14)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB15">
+    <cfRule type="expression" dxfId="73" priority="14">
+      <formula>AND($AB$15&lt;0.5,SUM($AB$15:$AB$16)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB16">
+    <cfRule type="expression" dxfId="72" priority="13">
+      <formula>AND($AB$16&lt;0.5,SUM($AB$15:$AB$16)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC5">
+    <cfRule type="expression" dxfId="71" priority="12">
+      <formula>AND($AC$5&lt;0.5,SUM($AC$5:$AC$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC6">
+    <cfRule type="expression" dxfId="70" priority="11">
+      <formula>AND($AC$6&lt;0.5,SUM($AC$5:$AC$6)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC7">
+    <cfRule type="expression" dxfId="69" priority="10">
+      <formula>AND($AC$7&lt;0.5,SUM($AC$7:$AC$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC8">
+    <cfRule type="expression" dxfId="68" priority="9">
+      <formula>AND($AC$8&lt;0.5,SUM($AC$7:$AC$8)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC9">
+    <cfRule type="expression" dxfId="67" priority="8">
+      <formula>AND($AC$9&lt;0.5,SUM($AC$9:$AC$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC10">
+    <cfRule type="expression" dxfId="66" priority="7">
+      <formula>AND($AC$10&lt;0.5,SUM($AC$9:$AC$10)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC11">
+    <cfRule type="expression" dxfId="65" priority="6">
+      <formula>AND($AC$11&lt;0.5,SUM($AC$11:$AC$12)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC12">
+    <cfRule type="expression" dxfId="64" priority="5">
+      <formula>AND($AC$12&lt;0.5,SUM($AC$11:$AC$12)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC13">
+    <cfRule type="expression" dxfId="63" priority="4">
+      <formula>AND($AC$13&lt;0.5,SUM($AC$13:$AC$14)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC14">
+    <cfRule type="expression" dxfId="62" priority="3">
+      <formula>AND($AC$14&lt;0.5,SUM($AC$13:$AC$14)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC15">
+    <cfRule type="expression" dxfId="61" priority="2">
+      <formula>AND($AC$15&lt;0.5,SUM($AC$15:$AC$16)&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC16">
+    <cfRule type="expression" dxfId="60" priority="1">
+      <formula>AND($AC$16&lt;0.5,SUM($AC$15:$AC$16)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>